<commit_message>
fix: fix test case
</commit_message>
<xml_diff>
--- a/src/__tests__/sample_xlsx/file_example_XLSX_50.xlsx
+++ b/src/__tests__/sample_xlsx/file_example_XLSX_50.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="205" firstSheet="0" activeTab="0"/>
+    <workbookView windowWidth="28800" windowHeight="13080" tabRatio="205"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115">
   <si>
     <t>First Name</t>
   </si>
@@ -366,127 +366,957 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+  <borders count="9">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
+    <cellStyle name="Total" xfId="24" builtinId="25"/>
+    <cellStyle name="Output" xfId="25" builtinId="21"/>
+    <cellStyle name="Currency" xfId="26" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Input" xfId="29" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
+    <cellStyle name="Good" xfId="32" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="Title" xfId="38" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
+    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
+    <cellStyle name="Link" xfId="43" builtinId="8"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K46" activeCellId="0" sqref="K46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="7"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1025" width="11.5178571428571"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="n">
+    <row r="1" s="1" customFormat="1" spans="1:8">
+      <c r="A1" s="1">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -511,1311 +1341,1310 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" spans="1:8">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>32</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2">
         <v>1562</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" spans="1:8">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>25</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>1582</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" spans="1:8">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>36</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4">
         <v>2587</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:8">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>25</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5">
         <v>3549</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" spans="1:8">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>58</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>2468</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" spans="1:8">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>24</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>2554</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" spans="1:8">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8">
         <v>56</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8">
         <v>3598</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+    <row r="9" spans="1:8">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9">
         <v>27</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9">
         <v>2456</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10">
         <v>40</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10">
         <v>6548</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="11" spans="1:8">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11">
         <v>28</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11">
         <v>5486</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+    <row r="12" spans="1:8">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12">
         <v>39</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12">
         <v>1258</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+    <row r="13" spans="1:8">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13">
         <v>38</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13">
         <v>2579</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+    <row r="14" spans="1:8">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14">
         <v>32</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14">
         <v>3256</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+    <row r="15" spans="1:8">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15">
         <v>26</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15">
         <v>2587</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+    <row r="16" spans="1:8">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16">
         <v>31</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16">
         <v>3259</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+    <row r="17" spans="1:8">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="0" t="s">
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17">
         <v>24</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="G17" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17">
         <v>1546</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+    <row r="18" spans="1:8">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="0" t="s">
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18">
         <v>39</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18">
         <v>3579</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+    <row r="19" spans="1:8">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="0" t="s">
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19">
         <v>28</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19">
         <v>6597</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+    <row r="20" spans="1:8">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20">
         <v>26</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="G20" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20">
         <v>9654</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+    <row r="21" spans="1:8">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21">
         <v>46</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G21" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21">
         <v>3569</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+    <row r="22" spans="1:8">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22">
         <v>37</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22">
         <v>2564</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+    <row r="23" spans="1:8">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23">
         <v>52</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="G23" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23">
         <v>8561</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+    <row r="24" spans="1:8">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="0" t="s">
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24">
         <v>46</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="G24" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24">
         <v>5489</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+    <row r="25" spans="1:8">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="0" t="s">
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25">
         <v>42</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="G25" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25">
         <v>5489</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+    <row r="26" spans="1:8">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26">
         <v>21</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26">
         <v>6574</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+    <row r="27" spans="1:8">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27">
         <v>28</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="G27" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27">
         <v>5555</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+    <row r="28" spans="1:8">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="0" t="s">
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28">
         <v>29</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="G28" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28">
         <v>6125</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+    <row r="29" spans="1:8">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="0" t="s">
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29">
         <v>23</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29">
         <v>5412</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+    <row r="30" spans="1:8">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30">
         <v>41</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="G30" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30">
         <v>3256</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+    <row r="31" spans="1:8">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31">
         <v>28</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="G31" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31">
         <v>3264</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+    <row r="32" spans="1:8">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" t="s">
         <v>76</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32">
         <v>37</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32">
         <v>4569</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+    <row r="33" spans="1:8">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="0" t="s">
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33">
         <v>34</v>
       </c>
-      <c r="G33" s="0" t="s">
+      <c r="G33" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="H33">
         <v>7521</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+    <row r="34" spans="1:8">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34">
         <v>26</v>
       </c>
-      <c r="G34" s="0" t="s">
+      <c r="G34" t="s">
         <v>20</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34">
         <v>6458</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+    <row r="35" spans="1:8">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="0" t="s">
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35">
         <v>35</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="G35" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35">
         <v>7569</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+    <row r="36" spans="1:8">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36">
         <v>36</v>
       </c>
-      <c r="G36" s="0" t="s">
+      <c r="G36" t="s">
         <v>20</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="H36">
         <v>8514</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+    <row r="37" spans="1:8">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37">
         <v>29</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="H37">
         <v>8563</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+    <row r="38" spans="1:8">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="0" t="s">
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="F38">
         <v>27</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="G38" t="s">
         <v>15</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="H38">
         <v>8642</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+    <row r="39" spans="1:8">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="0" t="s">
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="0" t="n">
+      <c r="F39">
         <v>25</v>
       </c>
-      <c r="G39" s="0" t="s">
+      <c r="G39" t="s">
         <v>20</v>
       </c>
-      <c r="H39" s="0" t="n">
+      <c r="H39">
         <v>9536</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+    <row r="40" spans="1:8">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="0" t="s">
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="F40">
         <v>36</v>
       </c>
-      <c r="G40" s="0" t="s">
+      <c r="G40" t="s">
         <v>20</v>
       </c>
-      <c r="H40" s="0" t="n">
+      <c r="H40">
         <v>2567</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+    <row r="41" spans="1:8">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" t="s">
         <v>94</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" t="s">
         <v>10</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="F41">
         <v>37</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="H41">
         <v>2154</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+    <row r="42" spans="1:8">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" t="s">
         <v>96</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" t="s">
         <v>18</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42">
         <v>26</v>
       </c>
-      <c r="G42" s="0" t="s">
+      <c r="G42" t="s">
         <v>15</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="H42">
         <v>3265</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+    <row r="43" spans="1:8">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" t="s">
         <v>98</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="0" t="s">
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="0" t="n">
+      <c r="F43">
         <v>37</v>
       </c>
-      <c r="G43" s="0" t="s">
+      <c r="G43" t="s">
         <v>20</v>
       </c>
-      <c r="H43" s="0" t="n">
+      <c r="H43">
         <v>8765</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+    <row r="44" spans="1:8">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" t="s">
         <v>100</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" t="s">
         <v>18</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" t="s">
         <v>19</v>
       </c>
-      <c r="F44" s="0" t="n">
+      <c r="F44">
         <v>24</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H44" s="0" t="n">
+      <c r="H44">
         <v>3259</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+    <row r="45" spans="1:8">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" t="s">
         <v>102</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="0" t="s">
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
         <v>10</v>
       </c>
-      <c r="F45" s="0" t="n">
+      <c r="F45">
         <v>39</v>
       </c>
-      <c r="G45" s="0" t="s">
+      <c r="G45" t="s">
         <v>15</v>
       </c>
-      <c r="H45" s="0" t="n">
+      <c r="H45">
         <v>3567</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+    <row r="46" spans="1:8">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" t="s">
         <v>104</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="0" t="n">
+      <c r="F46">
         <v>26</v>
       </c>
-      <c r="G46" s="0" t="s">
+      <c r="G46" t="s">
         <v>20</v>
       </c>
-      <c r="H46" s="0" t="n">
+      <c r="H46">
         <v>6540</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+    <row r="47" spans="1:8">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" t="s">
         <v>105</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" t="s">
         <v>106</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="0" t="s">
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
         <v>10</v>
       </c>
-      <c r="F47" s="0" t="n">
+      <c r="F47">
         <v>34</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H47" s="0" t="n">
+      <c r="H47">
         <v>2654</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+    <row r="48" spans="1:8">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" t="s">
         <v>107</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="0" t="s">
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="0" t="n">
+      <c r="F48">
         <v>28</v>
       </c>
-      <c r="G48" s="0" t="s">
+      <c r="G48" t="s">
         <v>15</v>
       </c>
-      <c r="H48" s="0" t="n">
+      <c r="H48">
         <v>6525</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+    <row r="49" spans="1:8">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" t="s">
         <v>109</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" t="s">
         <v>110</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="0" t="s">
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
         <v>10</v>
       </c>
-      <c r="F49" s="0" t="n">
+      <c r="F49">
         <v>32</v>
       </c>
-      <c r="G49" s="0" t="s">
+      <c r="G49" t="s">
         <v>20</v>
       </c>
-      <c r="H49" s="0" t="n">
+      <c r="H49">
         <v>3265</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
+    <row r="50" spans="1:8">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" t="s">
         <v>112</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" t="s">
         <v>18</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="E50" t="s">
         <v>10</v>
       </c>
-      <c r="F50" s="0" t="n">
+      <c r="F50">
         <v>39</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G50" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H50" s="0" t="n">
+      <c r="H50">
         <v>3265</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+    <row r="51" spans="1:8">
+      <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="0" t="s">
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s">
         <v>10</v>
       </c>
-      <c r="F51" s="0" t="n">
+      <c r="F51">
         <v>29</v>
       </c>
-      <c r="G51" s="0" t="s">
+      <c r="G51" t="s">
         <v>15</v>
       </c>
-      <c r="H51" s="0" t="n">
+      <c r="H51">
         <v>6125</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>